<commit_message>
Additional of solar calcs and RRT attempt
</commit_message>
<xml_diff>
--- a/uGrid_Input.xlsx
+++ b/uGrid_Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phy\Documents\OnePower\Python Models Local Copy\uGrid-master-GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8242916F-8277-4533-B2D3-0339233E21FE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{94DD6919-C783-4FE8-9319-00852D84CF33}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="2" xr2:uid="{68709F03-E2F0-4CA3-951F-ABB4DD9E87C4}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="PSO" sheetId="1" r:id="rId1"/>
     <sheet name="Econ" sheetId="2" r:id="rId2"/>
     <sheet name="Tech" sheetId="3" r:id="rId3"/>
+    <sheet name="Solar" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>maxGen</t>
   </si>
@@ -74,9 +75,6 @@
     <t>output_name</t>
   </si>
   <si>
-    <t>test1</t>
-  </si>
-  <si>
     <t>lifetime</t>
   </si>
   <si>
@@ -207,6 +205,48 @@
   </si>
   <si>
     <t>low_trip_perc</t>
+  </si>
+  <si>
+    <t>tariff_hillclimb_multiplier</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>timezone</t>
+  </si>
+  <si>
+    <t>slope</t>
+  </si>
+  <si>
+    <t>azimuth</t>
+  </si>
+  <si>
+    <t>pg</t>
+  </si>
+  <si>
+    <t>fpv</t>
+  </si>
+  <si>
+    <t>alpha_p</t>
+  </si>
+  <si>
+    <t>eff_mpp</t>
+  </si>
+  <si>
+    <t>repeatabilityTest3</t>
+  </si>
+  <si>
+    <t>f_inv</t>
+  </si>
+  <si>
+    <t>trans_losses</t>
   </si>
 </sst>
 </file>
@@ -560,11 +600,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{810FAEA2-4EF8-4AD5-9CE0-4B60A3CE1971}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -658,7 +714,7 @@
         <v>0.95</v>
       </c>
       <c r="O2" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -668,125 +724,128 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5ADBEA2-0E58-4F34-AFD4-59ED09832C5B}">
-  <dimension ref="A1:AJ2"/>
+  <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AK3" sqref="AK3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AE9" sqref="AE9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>23</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>24</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>27</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>28</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>29</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>30</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>32</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>33</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>34</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>35</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>36</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>37</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>38</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>39</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>40</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>41</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>42</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>43</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>44</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>45</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>46</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>47</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>48</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>49</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>50</v>
       </c>
-      <c r="AJ1" t="s">
-        <v>51</v>
+      <c r="AK1" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>15</v>
       </c>
@@ -895,6 +954,9 @@
       </c>
       <c r="AJ2">
         <v>1500</v>
+      </c>
+      <c r="AK2">
+        <v>1.01</v>
       </c>
     </row>
   </sheetData>
@@ -904,41 +966,44 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B00D0BC-366A-4E86-BC5F-EB05356D5715}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
         <v>52</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>53</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>54</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>55</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>56</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>57</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>58</v>
       </c>
-      <c r="H1" t="s">
-        <v>59</v>
+      <c r="I1" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>45</v>
       </c>
@@ -962,6 +1027,94 @@
       </c>
       <c r="H2">
         <v>0.05</v>
+      </c>
+      <c r="I2">
+        <v>0.08</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E26A88A2-799B-4631-B6FE-A8330968DD02}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2005</v>
+      </c>
+      <c r="B2">
+        <v>-33</v>
+      </c>
+      <c r="C2">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0.2</v>
+      </c>
+      <c r="H2">
+        <v>0.9</v>
+      </c>
+      <c r="I2">
+        <v>-2E-3</v>
+      </c>
+      <c r="J2">
+        <v>0.9</v>
+      </c>
+      <c r="K2">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First Final uGrid Net
fully completed uGrid Net codes with plots. Also updates to the uGrid code, there were some issues are not running from economic code. All fixed.
</commit_message>
<xml_diff>
--- a/uGrid_Input.xlsx
+++ b/uGrid_Input.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phy\Documents\OnePower\Python Models Local Copy\uGrid-master-GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF18897A-1F67-47C5-B798-932CDE9F14FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BD8C0F-EC04-4F04-9E63-B60229B56AE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="1" xr2:uid="{68709F03-E2F0-4CA3-951F-ABB4DD9E87C4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="4" xr2:uid="{68709F03-E2F0-4CA3-951F-ABB4DD9E87C4}"/>
   </bookViews>
   <sheets>
     <sheet name="PSO" sheetId="1" r:id="rId1"/>
     <sheet name="Econ" sheetId="2" r:id="rId2"/>
     <sheet name="Tech" sheetId="3" r:id="rId3"/>
     <sheet name="Solar" sheetId="4" r:id="rId4"/>
+    <sheet name="Net" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="82">
   <si>
     <t>maxGen</t>
   </si>
@@ -254,10 +255,31 @@
     <t>trans_losses</t>
   </si>
   <si>
-    <t>Cost_Dist_Board</t>
-  </si>
-  <si>
     <t>assuming $0.50/m</t>
+  </si>
+  <si>
+    <t>Cost_Trans_wire</t>
+  </si>
+  <si>
+    <t>reformatScaler</t>
+  </si>
+  <si>
+    <t>exclusionBuffer</t>
+  </si>
+  <si>
+    <t>MaxDistancePoleConn</t>
+  </si>
+  <si>
+    <t>minPoles</t>
+  </si>
+  <si>
+    <t>maxPoles</t>
+  </si>
+  <si>
+    <t>range_limit</t>
+  </si>
+  <si>
+    <t>repeats</t>
   </si>
 </sst>
 </file>
@@ -737,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5ADBEA2-0E58-4F34-AFD4-59ED09832C5B}">
   <dimension ref="A1:AL3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AD14" sqref="AD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -885,7 +907,7 @@
         <v>59</v>
       </c>
       <c r="AL1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.3">
@@ -1002,12 +1024,16 @@
         <v>1.01</v>
       </c>
       <c r="AL2">
-        <v>50</v>
+        <f>0.5*1000</f>
+        <v>500</v>
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.3">
       <c r="O3" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1171,4 +1197,74 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3256D70B-7508-42A8-AA62-A295C44165D1}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>70</v>
+      </c>
+      <c r="E2">
+        <v>85</v>
+      </c>
+      <c r="F2">
+        <v>500</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>